<commit_message>
New routing, now plots have unique ids and show_result() renders plots by ids. Also fixed redirection issue whe show_result() is triggered. Download button works. Plots ARE NOT deleted automatically!
</commit_message>
<xml_diff>
--- a/static/uploads/ICBGE_data.xlsx
+++ b/static/uploads/ICBGE_data.xlsx
@@ -1019,12 +1019,24 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1061,7 +1073,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1070,7 +1082,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1090,7 +1102,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1111,6 +1135,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF81D41A"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1227,8 +1311,8 @@
   </sheetPr>
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N33" activeCellId="0" sqref="N33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1516,48 +1600,48 @@
       <c r="A7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N7" s="1" t="n">
+      <c r="B7" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" s="8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="1" t="n">
@@ -1733,90 +1817,90 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N12" s="1" t="n">
+      <c r="B12" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" s="8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N13" s="1" t="n">
+      <c r="B13" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1909,90 +1993,90 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N16" s="1" t="n">
+      <c r="B16" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" s="8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N17" s="1" t="n">
+      <c r="B17" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N17" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2305,46 +2389,46 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J25" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M25" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N25" s="1" t="n">
+      <c r="B25" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N25" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2393,7 +2477,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B27" s="1" t="n">
@@ -2437,7 +2521,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="12" t="s">
         <v>40</v>
       </c>
       <c r="B28" s="1" t="n">
@@ -2481,7 +2565,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B29" s="1" t="n">
@@ -2525,7 +2609,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="12" t="s">
         <v>42</v>
       </c>
       <c r="B30" s="1" t="n">
@@ -2569,7 +2653,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B31" s="1" t="n">
@@ -2613,7 +2697,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="12" t="s">
         <v>44</v>
       </c>
       <c r="B32" s="1" t="n">
@@ -2657,7 +2741,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="9" t="s">
         <v>45</v>
       </c>
       <c r="B33" s="1" t="n">

</xml_diff>